<commit_message>
Correcion Excel Registrar Solicitud
</commit_message>
<xml_diff>
--- a/Service.MedicalRecord/wwwroot/layout/excel/expediente/InformeExpedientes.xlsx
+++ b/Service.MedicalRecord/wwwroot/layout/excel/expediente/InformeExpedientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanDanielGonzalezAl\Documents\Projects\API\Service.MedicalRecord\wwwroot\layout\excel\expediente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13332860-B977-45FF-A778-A6240F0C6337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088D298F-8413-4288-B029-0251D3D82183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
@@ -118,7 +118,7 @@
     </r>
   </si>
   <si>
-    <t>{{item.Status == 2 ? "Toma de Muestra" : "Solicitado"}}</t>
+    <t>{{item.NombreEstatus}}</t>
   </si>
 </sst>
 </file>
@@ -229,8 +229,124 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8497B0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8497B0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8497B0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8497B0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8497B0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8497B0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8497B0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8497B0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8497B0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8497B0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF8497B0"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -597,7 +713,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,6 +824,31 @@
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>"Clave"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+      <formula>"Nombre Estudio"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"Fecha de Registro"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>"Fecha de Entrega"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"Estatus"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
[Feat] => Descarga formato pdf Lista de Trabajo en Busqueda Masiva
</commit_message>
<xml_diff>
--- a/Service.MedicalRecord/wwwroot/layout/excel/expediente/InformeExpedientes.xlsx
+++ b/Service.MedicalRecord/wwwroot/layout/excel/expediente/InformeExpedientes.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanDanielGonzalezAl\Documents\Projects\API\Service.MedicalRecord\wwwroot\layout\excel\expediente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088D298F-8413-4288-B029-0251D3D82183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A589834A-57CD-4D86-A2D0-A643FB6174A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Expedientes" sheetId="1" r:id="rId1"/>
+    <sheet name="Solicitudes" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Expedientes">Expedientes!$A$4:$G$7</definedName>
-    <definedName name="Expedientes_Estudios">Expedientes!$A$5:$G$6</definedName>
+    <definedName name="Expedientes">Solicitudes!$A$4:$G$7</definedName>
+    <definedName name="Expedientes_Estudios">Solicitudes!$A$5:$G$6</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -229,62 +229,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8497B0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8497B0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8497B0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8497B0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8497B0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <b/>
@@ -713,7 +658,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,27 +770,27 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="B5">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Clave"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Nombre Estudio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Fecha de Registro"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Fecha de Entrega"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Estatus"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
[33902] Excel Toma de Muestra
</commit_message>
<xml_diff>
--- a/Service.MedicalRecord/wwwroot/layout/excel/expediente/InformeExpedientes.xlsx
+++ b/Service.MedicalRecord/wwwroot/layout/excel/expediente/InformeExpedientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanDanielGonzalezAl\Documents\Projects\API\Service.MedicalRecord\wwwroot\layout\excel\expediente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A589834A-57CD-4D86-A2D0-A643FB6174A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3BAACB-4D96-4C05-959B-53E16064F2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Solicitudes" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Expedientes">Solicitudes!$A$4:$G$7</definedName>
-    <definedName name="Expedientes_Estudios">Solicitudes!$A$5:$G$6</definedName>
+    <definedName name="Solicitudes">Solicitudes!$A$4:$G$7</definedName>
+    <definedName name="Solicitudes_Estudios">Solicitudes!$A$5:$G$6</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>

</xml_diff>